<commit_message>
feat: Arvore de decisões implementada
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>LIFE</t>
   </si>
@@ -36,30 +36,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>&gt;=1</t>
-  </si>
-  <si>
-    <t>&gt;=0</t>
-  </si>
-  <si>
-    <t>&lt;=2</t>
-  </si>
-  <si>
-    <t>&lt;100</t>
-  </si>
-  <si>
-    <t>&lt;=100</t>
-  </si>
-  <si>
-    <t>&gt;2</t>
-  </si>
-  <si>
-    <t>&gt;110</t>
-  </si>
-  <si>
-    <t>&lt;105</t>
-  </si>
-  <si>
     <t>ENEMY_COINS</t>
   </si>
   <si>
@@ -69,17 +45,41 @@
     <t>&gt;=800</t>
   </si>
   <si>
-    <t>&lt;=1</t>
-  </si>
-  <si>
-    <t>&lt;=0</t>
+    <t>&lt;3</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>&gt;=2</t>
+  </si>
+  <si>
+    <t>&lt;2</t>
+  </si>
+  <si>
+    <t>&gt;=60</t>
+  </si>
+  <si>
+    <t>&lt;60</t>
+  </si>
+  <si>
+    <t>&lt;300</t>
+  </si>
+  <si>
+    <t>&gt;=300</t>
+  </si>
+  <si>
+    <t>-1.5x7</t>
+  </si>
+  <si>
+    <t>0x7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -91,6 +91,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -115,12 +121,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -407,7 +416,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD17"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -433,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -441,62 +450,62 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>8</v>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Spawn de torres fixado
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>LIFE</t>
   </si>
@@ -39,18 +39,6 @@
     <t>ENEMY_COINS</t>
   </si>
   <si>
-    <t>&gt;=900</t>
-  </si>
-  <si>
-    <t>&gt;=800</t>
-  </si>
-  <si>
-    <t>&lt;3</t>
-  </si>
-  <si>
-    <t>&gt;=3</t>
-  </si>
-  <si>
     <t>&gt;=2</t>
   </si>
   <si>
@@ -73,6 +61,18 @@
   </si>
   <si>
     <t>0x7</t>
+  </si>
+  <si>
+    <t>1.5x7</t>
+  </si>
+  <si>
+    <t>-2.19x13.49</t>
+  </si>
+  <si>
+    <t>&gt;=500</t>
+  </si>
+  <si>
+    <t>&lt;500</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -130,6 +130,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -412,11 +415,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -450,62 +453,82 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Funções de Reset sendo chamadas corretamente
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>LIFE</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>&lt;500</t>
+  </si>
+  <si>
+    <t>-4,81x4,69</t>
   </si>
 </sst>
 </file>
@@ -415,11 +418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -531,6 +534,46 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: cenas organizadas no projeto
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>LIFE</t>
   </si>
@@ -39,12 +39,6 @@
     <t>ENEMY_COINS</t>
   </si>
   <si>
-    <t>&gt;=2</t>
-  </si>
-  <si>
-    <t>&lt;2</t>
-  </si>
-  <si>
     <t>&gt;=60</t>
   </si>
   <si>
@@ -57,32 +51,32 @@
     <t>&gt;=300</t>
   </si>
   <si>
-    <t>-1.5x7</t>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>BIG</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>-5x4.20</t>
+  </si>
+  <si>
+    <t>5x4.20</t>
   </si>
   <si>
     <t>0x7</t>
-  </si>
-  <si>
-    <t>1.5x7</t>
-  </si>
-  <si>
-    <t>-2.19x13.49</t>
-  </si>
-  <si>
-    <t>&gt;=500</t>
-  </si>
-  <si>
-    <t>&lt;500</t>
-  </si>
-  <si>
-    <t>-4,81x4,69</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,12 +88,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -124,15 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,11 +403,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD16"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -456,122 +441,62 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Arvore de decisões corrigida
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>LIFE</t>
   </si>
@@ -51,25 +51,31 @@
     <t>&gt;=300</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>BIG</t>
-  </si>
-  <si>
     <t>NORMAL</t>
   </si>
   <si>
     <t>FULL</t>
   </si>
   <si>
-    <t>-5x4.20</t>
-  </si>
-  <si>
     <t>5x4.20</t>
   </si>
   <si>
     <t>0x7</t>
+  </si>
+  <si>
+    <t>NORMAL_T</t>
+  </si>
+  <si>
+    <t>BIG_T</t>
+  </si>
+  <si>
+    <t>NORMAL_M</t>
+  </si>
+  <si>
+    <t>NONE_M</t>
+  </si>
+  <si>
+    <t>BIG_M</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -441,13 +447,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -456,18 +462,18 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -476,18 +482,18 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -496,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Projeto portado para android
</commit_message>
<xml_diff>
--- a/Assets/IA/towerSpawnerData.xlsx
+++ b/Assets/IA/towerSpawnerData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>LIFE</t>
   </si>
@@ -72,10 +72,28 @@
     <t>NORMAL_M</t>
   </si>
   <si>
+    <t>BIG_M</t>
+  </si>
+  <si>
+    <t>-5x4.20</t>
+  </si>
+  <si>
+    <t>NONE_T</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>-2x13</t>
+  </si>
+  <si>
+    <t>2x13</t>
+  </si>
+  <si>
     <t>NONE_M</t>
   </si>
   <si>
-    <t>BIG_M</t>
+    <t>5x12</t>
   </si>
 </sst>
 </file>
@@ -409,11 +427,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -459,50 +477,150 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>